<commit_message>
Update juoyter notebook for google colab test
</commit_message>
<xml_diff>
--- a/gap-replay/natural_and_alternative_heltcare/medicine_book_naturalhealtcare.xlsx
+++ b/gap-replay/natural_and_alternative_heltcare/medicine_book_naturalhealtcare.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Compartidos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RESEARCH\Hackaton_NLP_2024\SOURCE\SpanishMedicaLLM\gap-replay\natural_and_alternative_heltcare\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{346D902A-3296-4744-ABBD-DE7CA18FC254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20445" windowHeight="7680"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="75">
   <si>
     <t>Titulo</t>
   </si>
@@ -171,13 +172,91 @@
   </si>
   <si>
     <t xml:space="preserve">La Trofoterapia en la Medicina Tradicional China  Marcos Díaz Mastellari </t>
+  </si>
+  <si>
+    <t>LIBRO BLANCO de los herbolarios y las plantas medicinales</t>
+  </si>
+  <si>
+    <t>Fundación Salud y Naturaleza (S.N.)</t>
+  </si>
+  <si>
+    <t>España</t>
+  </si>
+  <si>
+    <t>https://www.fitoterapia.net/archivos/200701/260307libro-2.pdf?1</t>
+  </si>
+  <si>
+    <t>EL GRAN LIBRO DE LA MEDICINA CHINA</t>
+  </si>
+  <si>
+    <t>Ediciones URANO, S.A</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>http://bibliosjd.org/wp-content/uploads/2017/03/El-Gran-Libro-De-La-Medicina-China.pdf</t>
+  </si>
+  <si>
+    <t>EL GRAN LIBRO DE LA MEDICINA NATURAL</t>
+  </si>
+  <si>
+    <t>Ediciones Masters</t>
+  </si>
+  <si>
+    <t>Manual para la práctica de la Medicina Natural y Tradicional</t>
+  </si>
+  <si>
+    <t>Editorial Ciencias Médicas</t>
+  </si>
+  <si>
+    <t>https://instituciones.sld.cu/fcmdoct/files/2019/10/manual_medtrad_completo.pdf</t>
+  </si>
+  <si>
+    <t>Plantas medicinales de La Matamba y El Piñonal, municipio de Jamapa, Veracruz</t>
+  </si>
+  <si>
+    <t>Instituto de Ecología A. C. (INECOL)</t>
+  </si>
+  <si>
+    <t>978-607-7579-44-1</t>
+  </si>
+  <si>
+    <t>Plantas medicinales del Patio de Ángel albino corzo, chiaPas</t>
+  </si>
+  <si>
+    <t>Universidad Autónoma de Chiapas</t>
+  </si>
+  <si>
+    <t>978-607-561-075-7</t>
+  </si>
+  <si>
+    <t>https://editorial.unach.mx/documentos/digitales/_libs/plantasmedicinales.pdf</t>
+  </si>
+  <si>
+    <t>Contribución al conocimiento de las plantas medicinales del municipio de Tlatlauquitepec, Puebla</t>
+  </si>
+  <si>
+    <t>Ciencia Latina Revista Científica Multidisciplinar</t>
+  </si>
+  <si>
+    <t>10.37811/cl_rcm.v6i6.3741</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>CC BY 4.0</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/366057090_Contribucion_al_conocimiento_de_las_plantas_medicinales_del_municipio_de_Tlatlauquitepec_Puebla/fulltext/638fe03f484e65005bec8985/Contribucion-al-conocimiento-de-las-plantas-medicinales-del-municipio-de-Tlatlauquitepec-Puebla.pdf?origin=publicationDetail&amp;_sg%5B0%5D=jYRMsuvIrjqqIV7VxQZEe3Obc5lx6Wcjrg3H8wvQFc2L_h0oo1zJbHtAc67eIeE4-iOTkDSu5TJvuic_vLPYlg.yDBk41gY1IZGKVAVqqLEPnUKDcmcuieL78i_TRGXP80VwQHRFc-MmrCBUVWd8rrMrW90JOgQ97H1YH_w2XOP4Q&amp;_sg%5B1%5D=9UzfNT5FSWL9OpTEs5-JhJDupExQZDXmluX6173mQ-EvFoqvZ0_WfpxoYiD9-Z1mFjzIT2-_QmFnY2YHqWqCLhGeOXnrvIvmeal5h3AnsOlg.yDBk41gY1IZGKVAVqqLEPnUKDcmcuieL78i_TRGXP80VwQHRFc-MmrCBUVWd8rrMrW90JOgQ97H1YH_w2XOP4Q&amp;_iepl=&amp;_rtd=eyJjb250ZW50SW50ZW50IjoibWFpbkl0ZW0ifQ%3D%3D&amp;_tp=eyJjb250ZXh0Ijp7ImZpcnN0UGFnZSI6InB1YmxpY2F0aW9uIiwicGFnZSI6InB1YmxpY2F0aW9uIiwicG9zaXRpb24iOiJwYWdlSGVhZGVyIn19</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,6 +271,25 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="SabonLTStd-Roman"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -211,14 +309,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -496,24 +599,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
     <col min="4" max="4" width="72" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
-    <col min="6" max="7" width="18.28515625" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" customWidth="1"/>
+    <col min="6" max="7" width="18.33203125" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:12">
       <c r="C1" t="s">
         <v>37</v>
       </c>
@@ -543,7 +646,7 @@
       </c>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:12">
       <c r="C2">
         <v>1</v>
       </c>
@@ -554,7 +657,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:12">
       <c r="C3">
         <v>2</v>
       </c>
@@ -574,7 +677,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:12">
       <c r="C4">
         <v>3</v>
       </c>
@@ -582,7 +685,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:12">
       <c r="C5">
         <v>4</v>
       </c>
@@ -596,7 +699,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:12">
       <c r="C6">
         <v>5</v>
       </c>
@@ -616,7 +719,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:12">
       <c r="C7">
         <v>6</v>
       </c>
@@ -636,7 +739,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:12">
       <c r="C8">
         <v>7</v>
       </c>
@@ -647,7 +750,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:12">
       <c r="C9">
         <v>8</v>
       </c>
@@ -667,7 +770,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:12">
       <c r="C10">
         <v>9</v>
       </c>
@@ -684,7 +787,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:12">
       <c r="C11">
         <v>10</v>
       </c>
@@ -692,7 +795,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:12">
       <c r="C12">
         <v>11</v>
       </c>
@@ -712,7 +815,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:12">
       <c r="C13">
         <v>12</v>
       </c>
@@ -732,7 +835,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:12">
       <c r="C14">
         <v>13</v>
       </c>
@@ -743,7 +846,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:12">
       <c r="C15">
         <v>14</v>
       </c>
@@ -757,7 +860,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:12">
       <c r="C16">
         <v>15</v>
       </c>
@@ -768,7 +871,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:11">
       <c r="C17">
         <v>16</v>
       </c>
@@ -776,14 +879,165 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:11">
+      <c r="C18">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18">
+        <v>2007</v>
+      </c>
+      <c r="F18" t="s">
+        <v>50</v>
+      </c>
+      <c r="H18" t="s">
+        <v>51</v>
+      </c>
+      <c r="I18" t="s">
+        <v>37</v>
+      </c>
+      <c r="K18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11">
+      <c r="C19">
+        <v>18</v>
+      </c>
+      <c r="D19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19">
+        <v>2003</v>
+      </c>
+      <c r="F19" t="s">
+        <v>54</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" t="s">
+        <v>51</v>
+      </c>
+      <c r="I19" t="s">
+        <v>55</v>
+      </c>
+      <c r="K19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="3:11" ht="17.399999999999999">
+      <c r="C20">
+        <v>19</v>
+      </c>
+      <c r="D20" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="3:11">
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21">
+        <v>2014</v>
+      </c>
+      <c r="F21" t="s">
+        <v>60</v>
+      </c>
+      <c r="I21" t="s">
+        <v>55</v>
+      </c>
+      <c r="K21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" ht="14.25" customHeight="1">
+      <c r="C22">
+        <v>21</v>
+      </c>
+      <c r="D22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22">
+        <v>2015</v>
+      </c>
+      <c r="F22" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" t="s">
+        <v>64</v>
+      </c>
+      <c r="I22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11">
+      <c r="C23">
+        <v>22</v>
+      </c>
+      <c r="D23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23">
+        <v>2020</v>
+      </c>
+      <c r="F23" t="s">
+        <v>66</v>
+      </c>
+      <c r="H23" t="s">
+        <v>67</v>
+      </c>
+      <c r="I23" t="s">
+        <v>37</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11">
+      <c r="C24">
+        <v>23</v>
+      </c>
+      <c r="D24" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24">
+        <v>2022</v>
+      </c>
+      <c r="F24" t="s">
+        <v>70</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H24" t="s">
+        <v>72</v>
+      </c>
+      <c r="I24" t="s">
+        <v>73</v>
+      </c>
+      <c r="K24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11">
       <c r="C26" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G24" r:id="rId1" display="http://dx.doi.org/10.37811/cl_rcm.v6i6.3741" xr:uid="{9B312168-C62B-4EF1-A09C-8121D9B41E54}"/>
+    <hyperlink ref="K23" r:id="rId2" xr:uid="{7413816E-B048-41E4-B400-71C329680C2E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>